<commit_message>
Added more days for ordinary form
</commit_message>
<xml_diff>
--- a/static/documents/datedimension.xlsx
+++ b/static/documents/datedimension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsequeira/Python Projects/Ave Christus Rex/avechristusrex/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2DC985-4B49-A747-8E4B-584FC2639CFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1900EEFB-2C71-F64F-9A2F-C97469CBD96B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{7DAFA1EF-05D6-CA41-A437-56AA8F0EED2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Second</t>
   </si>
   <si>
-    <t>Sunday Cycle</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -333,9 +330,6 @@
     <t>Solemnity</t>
   </si>
   <si>
-    <t>A, B, C</t>
-  </si>
-  <si>
     <t>I, II</t>
   </si>
   <si>
@@ -388,6 +382,9 @@
   </si>
   <si>
     <t>Rose</t>
+  </si>
+  <si>
+    <t>Year Cycle</t>
   </si>
 </sst>
 </file>
@@ -761,7 +758,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38:K44"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,36 +783,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B16" si="0">YEAR(A2)</f>
@@ -830,28 +827,28 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
@@ -866,28 +863,28 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
@@ -902,28 +899,28 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
@@ -938,28 +935,28 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
@@ -974,28 +971,28 @@
         <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
@@ -1010,28 +1007,28 @@
         <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
@@ -1046,28 +1043,28 @@
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
@@ -1082,28 +1079,28 @@
         <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
@@ -1118,28 +1115,28 @@
         <v>20</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
@@ -1154,28 +1151,28 @@
         <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
@@ -1190,28 +1187,28 @@
         <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
@@ -1226,22 +1223,22 @@
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="4"/>
@@ -1249,7 +1246,7 @@
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
@@ -1264,28 +1261,28 @@
         <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
@@ -1300,28 +1297,28 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
@@ -1336,28 +1333,28 @@
         <v>26</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J16" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="4">
         <f>YEAR(A17)</f>
@@ -1372,32 +1369,32 @@
         <v>27</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" ref="B18:B44" si="3">YEAR(A18)</f>
@@ -1412,30 +1409,30 @@
         <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="3"/>
@@ -1450,30 +1447,30 @@
         <v>29</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="3"/>
@@ -1488,36 +1485,36 @@
         <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M20" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="3"/>
@@ -1532,30 +1529,30 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="3"/>
@@ -1570,30 +1567,30 @@
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" si="3"/>
@@ -1608,36 +1605,36 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="3"/>
@@ -1652,36 +1649,36 @@
         <v>4</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="3"/>
@@ -1696,30 +1693,30 @@
         <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="3"/>
@@ -1734,36 +1731,36 @@
         <v>6</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="3"/>
@@ -1778,36 +1775,36 @@
         <v>7</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="3"/>
@@ -1822,36 +1819,36 @@
         <v>8</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="4">
         <f t="shared" si="3"/>
@@ -1866,36 +1863,36 @@
         <v>9</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" si="3"/>
@@ -1910,30 +1907,30 @@
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="4">
         <f t="shared" si="3"/>
@@ -1948,36 +1945,36 @@
         <v>11</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="4">
         <f t="shared" si="3"/>
@@ -1992,30 +1989,30 @@
         <v>12</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="4">
         <f t="shared" si="3"/>
@@ -2030,36 +2027,36 @@
         <v>13</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="4">
         <f t="shared" si="3"/>
@@ -2074,36 +2071,36 @@
         <v>14</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="M34" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" s="4">
         <f t="shared" si="3"/>
@@ -2118,32 +2115,32 @@
         <v>15</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="4">
         <f t="shared" si="3"/>
@@ -2158,30 +2155,30 @@
         <v>16</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="4">
         <f t="shared" si="3"/>
@@ -2196,30 +2193,30 @@
         <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="4">
         <f t="shared" si="3"/>
@@ -2234,30 +2231,30 @@
         <v>18</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="4">
         <f t="shared" si="3"/>
@@ -2272,30 +2269,30 @@
         <v>19</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4">
         <f t="shared" si="3"/>
@@ -2310,30 +2307,30 @@
         <v>20</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="4">
         <f t="shared" si="3"/>
@@ -2348,30 +2345,30 @@
         <v>21</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="4">
         <f t="shared" si="3"/>
@@ -2386,30 +2383,30 @@
         <v>22</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4">
         <f t="shared" si="3"/>
@@ -2424,30 +2421,30 @@
         <v>23</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="4">
         <f t="shared" si="3"/>
@@ -2462,25 +2459,25 @@
         <v>24</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest fixes to New Liturgical Calendar
</commit_message>
<xml_diff>
--- a/static/documents/datedimension.xlsx
+++ b/static/documents/datedimension.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsequeira/Python Projects/Ave Christus Rex/avechristusrex/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1900EEFB-2C71-F64F-9A2F-C97469CBD96B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C24E2D2-A63E-E149-AC9A-C28E30A0BBD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{7DAFA1EF-05D6-CA41-A437-56AA8F0EED2D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{7DAFA1EF-05D6-CA41-A437-56AA8F0EED2D}"/>
   </bookViews>
   <sheets>
     <sheet name="datedimension" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -63,9 +63,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Weekday Cycle</t>
-  </si>
-  <si>
     <t>Qualifying Day</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>II</t>
-  </si>
-  <si>
     <t>Third</t>
   </si>
   <si>
@@ -354,9 +348,6 @@
     <t>Optional Memorial</t>
   </si>
   <si>
-    <t>St. Nicholar, Bishop</t>
-  </si>
-  <si>
     <t>St. Ambrose, Bishop and Doctor of the Church</t>
   </si>
   <si>
@@ -385,6 +376,39 @@
   </si>
   <si>
     <t>Year Cycle</t>
+  </si>
+  <si>
+    <t>Feast Short</t>
+  </si>
+  <si>
+    <t>St. Nicholas, Bishop</t>
+  </si>
+  <si>
+    <t>st-andrew</t>
+  </si>
+  <si>
+    <t>st-francis-xavier</t>
+  </si>
+  <si>
+    <t>st-john-damascene</t>
+  </si>
+  <si>
+    <t>st-nicholas</t>
+  </si>
+  <si>
+    <t>st-ambrose</t>
+  </si>
+  <si>
+    <t>immaculate-conception</t>
+  </si>
+  <si>
+    <t>st-juan-diego</t>
+  </si>
+  <si>
+    <t>st-damasus-i</t>
+  </si>
+  <si>
+    <t>st-lucy</t>
   </si>
 </sst>
 </file>
@@ -757,16 +781,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D552FDF1-F193-E245-A605-7FBF4F5DE2A7}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="59.33203125" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -783,36 +807,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
+        <v>113</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B16" si="0">YEAR(A2)</f>
@@ -827,28 +851,25 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
@@ -863,28 +884,25 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
@@ -899,28 +917,25 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
@@ -935,28 +950,25 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
@@ -971,28 +983,25 @@
         <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
@@ -1007,28 +1016,25 @@
         <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
@@ -1043,28 +1049,25 @@
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
@@ -1079,28 +1082,25 @@
         <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
@@ -1115,28 +1115,25 @@
         <v>20</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
@@ -1151,28 +1148,25 @@
         <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
@@ -1187,28 +1181,25 @@
         <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
@@ -1223,30 +1214,28 @@
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
@@ -1261,28 +1250,25 @@
         <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
@@ -1297,28 +1283,25 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
@@ -1333,28 +1316,25 @@
         <v>26</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="4">
         <f>YEAR(A17)</f>
@@ -1369,32 +1349,30 @@
         <v>27</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>98</v>
+      <c r="I17" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>114</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" ref="B18:B44" si="3">YEAR(A18)</f>
@@ -1409,30 +1387,27 @@
         <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>98</v>
+      <c r="I18" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="3"/>
@@ -1447,30 +1422,27 @@
         <v>29</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="3"/>
@@ -1485,36 +1457,36 @@
         <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="3"/>
@@ -1529,30 +1501,27 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="3"/>
@@ -1567,30 +1536,27 @@
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" si="3"/>
@@ -1605,36 +1571,36 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="M23" s="4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="3"/>
@@ -1649,36 +1615,36 @@
         <v>4</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>98</v>
+      <c r="I24" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="3"/>
@@ -1693,30 +1659,27 @@
         <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="3"/>
@@ -1731,36 +1694,36 @@
         <v>6</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="3"/>
@@ -1775,36 +1738,36 @@
         <v>7</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="M27" s="4" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="3"/>
@@ -1819,36 +1782,36 @@
         <v>8</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="4">
         <f t="shared" si="3"/>
@@ -1863,36 +1826,36 @@
         <v>9</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" si="3"/>
@@ -1907,30 +1870,27 @@
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="4">
         <f t="shared" si="3"/>
@@ -1945,36 +1905,36 @@
         <v>11</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>98</v>
+      <c r="I31" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="4">
         <f t="shared" si="3"/>
@@ -1989,30 +1949,27 @@
         <v>12</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" s="4">
         <f t="shared" si="3"/>
@@ -2027,36 +1984,36 @@
         <v>13</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L33" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="M33" s="4" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4">
         <f t="shared" si="3"/>
@@ -2071,36 +2028,34 @@
         <v>14</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L34" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B35" s="4">
         <f t="shared" si="3"/>
@@ -2115,32 +2070,30 @@
         <v>15</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>115</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B36" s="4">
         <f t="shared" si="3"/>
@@ -2155,30 +2108,27 @@
         <v>16</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4">
         <f t="shared" si="3"/>
@@ -2193,30 +2143,27 @@
         <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" s="4">
         <f t="shared" si="3"/>
@@ -2231,30 +2178,27 @@
         <v>18</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>98</v>
+      <c r="I38" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B39" s="4">
         <f t="shared" si="3"/>
@@ -2269,30 +2213,27 @@
         <v>19</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B40" s="4">
         <f t="shared" si="3"/>
@@ -2307,30 +2248,27 @@
         <v>20</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" s="4">
         <f t="shared" si="3"/>
@@ -2345,30 +2283,27 @@
         <v>21</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B42" s="4">
         <f t="shared" si="3"/>
@@ -2383,30 +2318,27 @@
         <v>22</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" s="4">
         <f t="shared" si="3"/>
@@ -2421,30 +2353,27 @@
         <v>23</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B44" s="4">
         <f t="shared" si="3"/>
@@ -2459,25 +2388,22 @@
         <v>24</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest updates to Daily Liturgy
</commit_message>
<xml_diff>
--- a/static/documents/datedimension.xlsx
+++ b/static/documents/datedimension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsequeira/Python Projects/Ave Christus Rex/avechristusrex/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E65666-8D96-4549-B0FC-A1AABD00B3F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11453B85-C402-4D4C-B402-EE201927A1BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{7DAFA1EF-05D6-CA41-A437-56AA8F0EED2D}"/>
   </bookViews>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D552FDF1-F193-E245-A605-7FBF4F5DE2A7}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,6 +810,8 @@
     <col min="9" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="59.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Latest changes - Added Lenten base
</commit_message>
<xml_diff>
--- a/static/documents/datedimension.xlsx
+++ b/static/documents/datedimension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsequeira/Python Projects/Ave Christus Rex/avechristusrex/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA9DFBC-AC80-F642-BD45-D4FB5411B206}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A94A2D0-6D8E-5F44-BF75-2B132C67CEC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{7DAFA1EF-05D6-CA41-A437-56AA8F0EED2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="346">
   <si>
     <t>Date</t>
   </si>
@@ -1066,6 +1066,12 @@
   </si>
   <si>
     <t>2023-03-31</t>
+  </si>
+  <si>
+    <t>Ash Wednesday</t>
+  </si>
+  <si>
+    <t>ashwednesday</t>
   </si>
 </sst>
 </file>
@@ -1438,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D552FDF1-F193-E245-A605-7FBF4F5DE2A7}">
   <dimension ref="A1:R141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6542,7 +6548,7 @@
         <v>310</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>179</v>
@@ -6550,8 +6556,14 @@
       <c r="J104" s="4" t="s">
         <v>254</v>
       </c>
+      <c r="K104" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="M104" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="O104" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -6580,13 +6592,16 @@
         <v>310</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>179</v>
       </c>
       <c r="J105" s="4" t="s">
         <v>254</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="M105" s="1" t="s">
         <v>111</v>
@@ -6618,13 +6633,16 @@
         <v>310</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="I106" s="4" t="s">
         <v>179</v>
       </c>
       <c r="J106" s="4" t="s">
         <v>254</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="M106" s="1" t="s">
         <v>111</v>
@@ -6656,13 +6674,16 @@
         <v>310</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="I107" s="4" t="s">
         <v>179</v>
       </c>
       <c r="J107" s="4" t="s">
         <v>254</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="M107" s="1" t="s">
         <v>111</v>

</xml_diff>